<commit_message>
Adding Unique Event Documents
</commit_message>
<xml_diff>
--- a/data/Study_01/Raw/Unique_Events_Pilot.xlsx
+++ b/data/Study_01/Raw/Unique_Events_Pilot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wjpmi\Documents\GitHub\fright_night_study\data\Study_01\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wjpmi\Documents\GitHub\fright_night_study\Data\Study_01\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA37EC09-47DB-4D81-A1AA-E6F7CA20BF7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CF6A61-4E9A-4385-876B-CC5A11436755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="15800" xr2:uid="{96F388A5-19E8-4834-8DAF-0A764BF7587D}"/>
+    <workbookView xWindow="-28800" yWindow="2115" windowWidth="14400" windowHeight="15600" xr2:uid="{96F388A5-19E8-4834-8DAF-0A764BF7587D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -304,10 +304,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -629,20 +625,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7246218E-A98C-44A6-8A6F-391067A0A667}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="17.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,7 +669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -687,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -701,7 +697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -715,7 +711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -729,7 +725,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
@@ -743,7 +739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
@@ -757,7 +753,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -771,7 +767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -785,7 +781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -799,7 +795,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -813,7 +809,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -827,7 +823,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -841,7 +837,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -855,7 +851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -869,7 +865,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -883,7 +879,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -897,7 +893,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -911,7 +907,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -925,7 +921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
@@ -939,7 +935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>61</v>
       </c>
@@ -953,7 +949,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -967,7 +963,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="55.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>